<commit_message>
latest calculations in component selection
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070EBD2C-A515-4B85-AF1A-444461CCB77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB047647-8F75-4078-86BB-00DA7418D54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,6 +52,30 @@
           </rPr>
           <t>S. Riggleman:
 For 8 bit PWM Resolution, fPWM = ~280kHz</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{8B9B384E-B41C-4BEF-9229-1A0C397CF8FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows PC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note on operating in DCM vs CCM:https://electronics.stackexchange.com/questions/571412/how-does-the-inductor-current-ripple-influence-a-switch-mode-power-supply</t>
         </r>
       </text>
     </comment>
@@ -98,12 +123,105 @@
         </r>
       </text>
     </comment>
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{9E58D6B8-560A-4477-B10C-5AA42D61DA6B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S.Riggleman</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Taken from coilcraft's loss comparison: https://www.coilcraft.com/en-us/tools/power-inductor-finder/#/search</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Windows PC</author>
+  </authors>
+  <commentList>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{2D1EC2AE-CC7C-4BD7-84F4-845D7952BDBB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+For 8 bit PWM Resolution, fPWM = ~280kHz</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{C4099B91-925B-41D4-9B85-E89E56DD8467}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman: 50% comes from diminishing returns of shrinking inductor past ripple value &gt; 50% of avg current</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{9C46298D-4685-499D-BDB6-2DBA9B561428}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+Chose as opposed to D2-Pak package due to chip shortage - 4200 available on Mouser and interchangable if necessary</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{6AAF341F-B55A-4B61-8CB2-CEC34DBF6D7D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+The Total Gate Charge (Qg) is the amount of charge that needs to be injected into the gate electrode to turn ON (drive) the MOSFET.
+https://www.rohm.com/electronics-basics/transistors/total-gate-charge</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -165,9 +283,6 @@
     <t xml:space="preserve">Phase output current:  </t>
   </si>
   <si>
-    <t>Phase input current:</t>
-  </si>
-  <si>
     <t>Component Selection &amp; Losses</t>
   </si>
   <si>
@@ -183,9 +298,6 @@
     <t>Total Output power:</t>
   </si>
   <si>
-    <t>Inductor Value:</t>
-  </si>
-  <si>
     <t>Switching Frequency Per Phase:</t>
   </si>
   <si>
@@ -274,13 +386,28 @@
   </si>
   <si>
     <t>Qoss Losses Per FET:</t>
+  </si>
+  <si>
+    <t>Ballpark Inductor Value:</t>
+  </si>
+  <si>
+    <t>Phase avg input current:</t>
+  </si>
+  <si>
+    <t>VER2923-223</t>
+  </si>
+  <si>
+    <t>Core + Winding Losses Per Phase(W):</t>
+  </si>
+  <si>
+    <t>Total Core Losses (W)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +462,19 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -357,14 +497,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,11 +506,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,8 +841,452 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>450000</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="J7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <f>E7/E9</f>
+        <v>225000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <f>E13*0.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8">
+        <f>SQRT(E10)*E13</f>
+        <v>6.3160509814281891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>48.72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9">
+        <f>(B16*E10)/(H8*E8)</f>
+        <v>2.3698370370370368E-5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9">
+        <f>SQRT(1-E10)*E13</f>
+        <v>6.4115130819487538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <f>(B18-B16)/B18</f>
+        <v>0.49249999999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <f>(H8/2) + E13</f>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <f>E11*B19</f>
+        <v>833.11199999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13">
+        <f>(B17/E9)</f>
+        <v>9</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <f>(E12/E9)/B18</f>
+        <v>4.3391250000000001</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <f>22*POWER(10,-6)</f>
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f>B9</f>
+        <v>48.72</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16">
+        <f>100*POWER(10,-9)</f>
+        <v>1.0000000000000001E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f>B8*B10</f>
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17">
+        <v>14.7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17">
+        <f>299*POWER(10,-9)</f>
+        <v>2.9900000000000002E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>B13</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <f>B16*B17</f>
+        <v>876.96</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20">
+        <f>(B16*E10)/(H15*E8)</f>
+        <v>4.8473939393939389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21">
+        <f>E13+(0.5*H20)</f>
+        <v>11.423696969696969</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22">
+        <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
+        <v>9.1081338557159679</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23">
+        <f>POWER(H22,2)*H16</f>
+        <v>0.21569106606746252</v>
+      </c>
+      <c r="J23" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23">
+        <f>POWER(K8,2)*K15</f>
+        <v>0.17951624999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24">
+        <f>H23*E9</f>
+        <v>0.43138213213492504</v>
+      </c>
+      <c r="J24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24">
+        <f>POWER(K9,2)*K15</f>
+        <v>0.18498375000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25">
+        <v>1.619</v>
+      </c>
+      <c r="J25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25">
+        <f>SUM(K23:K24)*E9</f>
+        <v>0.72899999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26">
+        <f>H25*E9</f>
+        <v>3.238</v>
+      </c>
+      <c r="J26" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26">
+        <f>B18*E13*10*POWER(10,-9)*E8</f>
+        <v>1.9440000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J27" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27">
+        <f>K26*E9</f>
+        <v>3.8880000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28">
+        <f>(K17/2)*B18*E8</f>
+        <v>3.2292000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K14" r:id="rId1" xr:uid="{1BC3AC28-62FC-4FF1-971A-2FE9F728A67C}"/>
+    <hyperlink ref="H14" r:id="rId2" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F195F5-CEE8-422B-8C7F-84AE41425DAF}">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,20 +1300,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -737,44 +1324,44 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7">
-        <v>280000</v>
+        <v>250000</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="H7" s="7"/>
       <c r="J7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -784,25 +1371,25 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <f>E7/E9</f>
-        <v>140000</v>
+        <v>125000</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <f>E13*0.5</f>
-        <v>4.5</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K8">
         <f>SQRT(E10)*E13</f>
-        <v>6.3160509814281891</v>
+        <v>4.7444045991040857</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -819,18 +1406,18 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="H9">
-        <f>(B16*E10)/(H8*E7)</f>
-        <v>1.9043333333333331E-5</v>
+        <f>(B16*E10)/(H8*E8)</f>
+        <v>1.26984126984127E-5</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K9">
         <f>SQRT(1-E10)*E13</f>
-        <v>6.4115130819487538</v>
+        <v>5.613655226320903</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -845,14 +1432,14 @@
       </c>
       <c r="E10">
         <f>(B18-B16)/B18</f>
-        <v>0.49249999999999999</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10">
         <f>(H8/2) + E13</f>
-        <v>11.25</v>
+        <v>9.1875</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -864,15 +1451,15 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <f>E11*B19</f>
-        <v>833.11199999999997</v>
+        <v>195.50999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -883,20 +1470,20 @@
         <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="E13">
         <f>(B17/E9)</f>
-        <v>9</v>
+        <v>7.35</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
@@ -904,34 +1491,34 @@
       </c>
       <c r="E14">
         <f>(E12/E9)/B18</f>
-        <v>4.3391250000000001</v>
+        <v>4.0731249999999992</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
         <v>29</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
       </c>
       <c r="H15">
         <f>22*POWER(10,-6)</f>
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K15">
         <v>4.4999999999999997E-3</v>
@@ -942,17 +1529,16 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <f>B9</f>
-        <v>48.72</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H16">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="J16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K16">
         <f>100*POWER(10,-9)</f>
@@ -964,17 +1550,16 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <f>B8*B10</f>
-        <v>18</v>
+        <v>14.7</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H17">
         <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K17">
         <f>299*POWER(10,-9)</f>
@@ -986,144 +1571,143 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <f>B13</f>
-        <v>96</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <f>B16*B17</f>
-        <v>876.96</v>
+        <v>205.79999999999998</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20">
+        <f>(B16*E10)/(H15*E8)</f>
+        <v>2.1212121212121215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G21" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="H19" s="6"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G20" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20">
-        <f>(B16*E10)/(H15*E7)</f>
-        <v>3.8952272727272725</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G21" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="H21">
         <f>E13+(0.5*H20)</f>
-        <v>10.947613636363636</v>
+        <v>8.4106060606060602</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G22" s="8" t="s">
-        <v>43</v>
+      <c r="G22" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="H22">
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
-        <v>9.0699724159181727</v>
+        <v>7.375463493137099</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G23" s="8" t="s">
-        <v>39</v>
+      <c r="G23" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="H23">
         <f>POWER(H22,2)*H16</f>
-        <v>0.21388743902634297</v>
+        <v>0.14143340052035505</v>
       </c>
       <c r="J23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K23">
         <f>POWER(K8,2)*K15</f>
-        <v>0.17951624999999996</v>
+        <v>0.10129218750000001</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G24" s="8" t="s">
-        <v>40</v>
+      <c r="G24" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="H24">
         <f>H23*E9</f>
-        <v>0.42777487805268594</v>
+        <v>0.2828668010407101</v>
       </c>
       <c r="J24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K24">
         <f>POWER(K9,2)*K15</f>
-        <v>0.18498375000000003</v>
+        <v>0.14180906249999994</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G25" s="8" t="s">
-        <v>41</v>
+      <c r="G25" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="J25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K25">
         <f>SUM(K23:K24)*E9</f>
-        <v>0.72899999999999998</v>
+        <v>0.48620249999999987</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G26" s="8" t="s">
-        <v>42</v>
+      <c r="G26" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="J26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K26">
-        <f>B18*E13*POWER(10,-9)*E7</f>
-        <v>0.24192</v>
+        <f>B18*E13*10*POWER(10,-9)*E8</f>
+        <v>0.2205</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K27">
         <f>K26*E9</f>
-        <v>0.48383999999999999</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K28">
         <f>(K17/2)*B18*E7</f>
-        <v>4.0185599999999999</v>
+        <v>0.89700000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="G13:H13"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J13:K13"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:N5"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1" display="https://www.coilcraft.com/en-us/products/power/shielded-inductors/high-current-flat-wire/ser/ser29xx/?skuId=10177" xr:uid="{0EE49C7A-D2F0-4E00-8950-1D677D5C1245}"/>
-    <hyperlink ref="K14" r:id="rId2" xr:uid="{1BC3AC28-62FC-4FF1-971A-2FE9F728A67C}"/>
+    <hyperlink ref="H14" r:id="rId1" display="https://www.coilcraft.com/en-us/products/power/shielded-inductors/high-current-flat-wire/ser/ser29xx/?skuId=10177" xr:uid="{B9E7DE04-5BE9-4709-A171-D1A5F059421D}"/>
+    <hyperlink ref="K14" r:id="rId2" xr:uid="{F6CD9C4B-A3B0-43B4-9E7F-23B8D2A7A72B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
fix gate charge and switching losses calcs, pick gate driver
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB047647-8F75-4078-86BB-00DA7418D54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA66DA2C-753C-44C1-84B0-FF4E737358A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
@@ -108,6 +108,22 @@
         </r>
       </text>
     </comment>
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{2DB8DF83-E7F4-4A3F-9C74-F723186D2C43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby R:
+Excellent resource on gate charge characteristics: 
+https://www.microsemi.com/document-portal/doc_view/14697-making-use-of-gate-charge-information-in-mosfet-and-igbt-data-sheets</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K16" authorId="0" shapeId="0" xr:uid="{AA3543EF-7AE4-4048-8AB5-AC00A783E811}">
       <text>
         <r>
@@ -120,6 +136,36 @@
           <t>S. Riggleman:
 The Total Gate Charge (Qg) is the amount of charge that needs to be injected into the gate electrode to turn ON (drive) the MOSFET.
 https://www.rohm.com/electronics-basics/transistors/total-gate-charge</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{9F4733D5-1342-4FFD-8C3F-576434C79316}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby R:
+This is the charge that is relevant for switching losses = Qgd + (Qg-Qgd-Qgth)=Qsw</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{8FE40EFA-1036-474F-AB52-47115A34EEBB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Helpful page on benefits of low Qrr:
+https://efficiencywins.nexperia.com/efficient-products/qrr-overlooked-and-underappreciated-in-efficiency-battle.html</t>
         </r>
       </text>
     </comment>
@@ -221,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -401,6 +447,27 @@
   </si>
   <si>
     <t>Total Core Losses (W)</t>
+  </si>
+  <si>
+    <t>Qrr</t>
+  </si>
+  <si>
+    <t>Switching Charge (Coul.)</t>
+  </si>
+  <si>
+    <t>FET Driver</t>
+  </si>
+  <si>
+    <t>Source/Sink Current</t>
+  </si>
+  <si>
+    <t>Turn on time (S)</t>
+  </si>
+  <si>
+    <t>MIC4102</t>
+  </si>
+  <si>
+    <t>Design for MIC4102 for PWM input, add a not gate that can be DNP normally, but populated if need to change dot MIC4103</t>
   </si>
 </sst>
 </file>
@@ -839,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -853,9 +920,10 @@
     <col min="8" max="8" width="11.453125" customWidth="1"/>
     <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -864,14 +932,14 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -879,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -899,7 +967,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -918,8 +986,14 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -947,8 +1021,14 @@
         <f>SQRT(E10)*E13</f>
         <v>6.3160509814281891</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -976,7 +1056,7 @@
         <v>6.4115130819487538</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -998,15 +1078,21 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="E11">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1018,7 +1104,7 @@
         <v>833.11199999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1041,7 +1127,7 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -1062,7 +1148,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1080,7 +1166,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1098,8 +1184,8 @@
         <v>52</v>
       </c>
       <c r="K16">
-        <f>100*POWER(10,-9)</f>
-        <v>1.0000000000000001E-7</v>
+        <f>80*POWER(10,-9)</f>
+        <v>8.0000000000000002E-8</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1117,11 +1203,11 @@
         <v>14.7</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="K17">
-        <f>299*POWER(10,-9)</f>
-        <v>2.9900000000000002E-7</v>
+        <f>26*POWER(10,-9)</f>
+        <v>2.6000000000000001E-8</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1132,6 +1218,13 @@
         <f>B13</f>
         <v>96</v>
       </c>
+      <c r="J18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18">
+        <f>299*POWER(10,-9)</f>
+        <v>2.9900000000000002E-7</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1145,7 +1238,9 @@
         <v>34</v>
       </c>
       <c r="H19" s="6"/>
-      <c r="J19" s="1"/>
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G20" s="5" t="s">
@@ -1155,6 +1250,13 @@
         <f>(B16*E10)/(H15*E8)</f>
         <v>4.8473939393939389</v>
       </c>
+      <c r="J20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20">
+        <f>K17/N11</f>
+        <v>8.6666666666666665E-9</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G21" s="5" t="s">
@@ -1237,8 +1339,8 @@
         <v>50</v>
       </c>
       <c r="K26">
-        <f>B18*E13*10*POWER(10,-9)*E8</f>
-        <v>1.9440000000000002</v>
+        <f>B18*E13*K20*E8</f>
+        <v>1.6848000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -1247,7 +1349,7 @@
       </c>
       <c r="K27">
         <f>K26*E9</f>
-        <v>3.8880000000000003</v>
+        <v>3.3696000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -1255,12 +1357,12 @@
         <v>54</v>
       </c>
       <c r="K28">
-        <f>(K17/2)*B18*E8</f>
+        <f>(K18/2)*B18*E8</f>
         <v>3.2292000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="J13:K13"/>
@@ -1270,6 +1372,7 @@
     <mergeCell ref="G5:N5"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:P7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{1BC3AC28-62FC-4FF1-971A-2FE9F728A67C}"/>

</xml_diff>

<commit_message>
add design process document, also change design to three string single phases with different inductor for lower switching freqency and switching losses
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA66DA2C-753C-44C1-84B0-FF4E737358A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C99689-4BE4-4098-92E0-900B7635296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Multi_String_Single_phase" sheetId="3" r:id="rId1"/>
+    <sheet name="Original_Multiphase" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
     <author>Windows PC</author>
   </authors>
   <commentList>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{5FBF964B-8E52-42FE-A1BE-4091C63B5871}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{C4638315-B48B-48DE-A9B9-BE8E74762BF5}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{8B9B384E-B41C-4BEF-9229-1A0C397CF8FF}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{6B63245F-A5B5-4702-BCAA-725EB06F4476}">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{B0EC1784-8AED-4914-90B7-5529A0924461}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{08DDFE2B-2AFC-4708-BBE9-AA4783C690C1}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{99931F6F-1D2B-4A35-AFF8-CFF17CC6F28A}">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{2D072AD2-0612-4777-9B01-271BE2591622}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby R:
+Alternative Part option:PA4349.104ANLT
+Wurth chosen because of AC loss simulator</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{7798945C-4F58-4F6F-9D7D-36AC90095635}">
       <text>
         <r>
           <rPr>
@@ -108,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{2DB8DF83-E7F4-4A3F-9C74-F723186D2C43}">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{AAB8FCD8-8C36-4300-9FE2-D2B8A04F511B}">
       <text>
         <r>
           <rPr>
@@ -124,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{AA3543EF-7AE4-4048-8AB5-AC00A783E811}">
+    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{19BC1F6C-6807-49CB-8B63-D435A2E1D5B0}">
       <text>
         <r>
           <rPr>
@@ -139,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{9F4733D5-1342-4FFD-8C3F-576434C79316}">
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{E03F4A58-934D-4F90-BDBE-944945276722}">
       <text>
         <r>
           <rPr>
@@ -154,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{8FE40EFA-1036-474F-AB52-47115A34EEBB}">
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{CC48B0D2-67F7-4335-82FC-5FA63D01D5B7}">
       <text>
         <r>
           <rPr>
@@ -169,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{9E58D6B8-560A-4477-B10C-5AA42D61DA6B}">
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{C6BCF19B-A17F-42C4-8FCB-0C6CA1CFAAA6}">
       <text>
         <r>
           <rPr>
@@ -189,7 +205,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Taken from coilcraft's loss comparison: https://www.coilcraft.com/en-us/tools/power-inductor-finder/#/search</t>
+Taken from Wurth Loss calculator: https://redexpert.we-online.com/redexpert/#/module/7104/selecteditems/74437529203101/productdata/=74437529203101/type/+or+Single+Single_HV/Ir/gte:6A/Tris/lte:80K/Isat/gte:7.5A/applicationbar/LossCalculator/on/frequency/80kHz+0.5/inductorType/Single+Suitable/winding1/6A+DeltaIA+3A+2V+-2V
+</t>
         </r>
       </text>
     </comment>
@@ -203,7 +220,7 @@
     <author>Windows PC</author>
   </authors>
   <commentList>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{2D1EC2AE-CC7C-4BD7-84F4-845D7952BDBB}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{5FBF964B-8E52-42FE-A1BE-4091C63B5871}">
       <text>
         <r>
           <rPr>
@@ -218,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{C4099B91-925B-41D4-9B85-E89E56DD8467}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{8B9B384E-B41C-4BEF-9229-1A0C397CF8FF}">
       <text>
         <r>
           <rPr>
@@ -228,11 +245,35 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>S. Riggleman: 50% comes from diminishing returns of shrinking inductor past ripple value &gt; 50% of avg current</t>
+          <t>Windows PC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note on operating in DCM vs CCM:https://electronics.stackexchange.com/questions/571412/how-does-the-inductor-current-ripple-influence-a-switch-mode-power-supply</t>
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{9C46298D-4685-499D-BDB6-2DBA9B561428}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{B0EC1784-8AED-4914-90B7-5529A0924461}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman: 50% comes from diminishing returns of shrinking inductor past ripple value &gt; 50% of avg current</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{99931F6F-1D2B-4A35-AFF8-CFF17CC6F28A}">
       <text>
         <r>
           <rPr>
@@ -247,7 +288,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{6AAF341F-B55A-4B61-8CB2-CEC34DBF6D7D}">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{2DB8DF83-E7F4-4A3F-9C74-F723186D2C43}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby R:
+Excellent resource on gate charge characteristics: 
+https://www.microsemi.com/document-portal/doc_view/14697-making-use-of-gate-charge-information-in-mosfet-and-igbt-data-sheets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{AA3543EF-7AE4-4048-8AB5-AC00A783E811}">
       <text>
         <r>
           <rPr>
@@ -259,6 +316,60 @@
           <t>S. Riggleman:
 The Total Gate Charge (Qg) is the amount of charge that needs to be injected into the gate electrode to turn ON (drive) the MOSFET.
 https://www.rohm.com/electronics-basics/transistors/total-gate-charge</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{9F4733D5-1342-4FFD-8C3F-576434C79316}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shelby R:
+This is the charge that is relevant for switching losses = Qgd + (Qg-Qgd-Qgth)=Qsw</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{8FE40EFA-1036-474F-AB52-47115A34EEBB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Helpful page on benefits of low Qrr:
+https://efficiencywins.nexperia.com/efficient-products/qrr-overlooked-and-underappreciated-in-efficiency-battle.html</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{9E58D6B8-560A-4477-B10C-5AA42D61DA6B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S.Riggleman</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Taken from coilcraft's loss comparison: https://www.coilcraft.com/en-us/tools/power-inductor-finder/#/search</t>
         </r>
       </text>
     </comment>
@@ -267,7 +378,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -362,9 +473,6 @@
     <t xml:space="preserve">Part Number: </t>
   </si>
   <si>
-    <t>SER2918H-223</t>
-  </si>
-  <si>
     <t>DCR (Ohm):</t>
   </si>
   <si>
@@ -386,21 +494,12 @@
     <t>Total DCR Losses(W)</t>
   </si>
   <si>
-    <t>Core Losses Per Phase(W):</t>
-  </si>
-  <si>
-    <t>Total Core Losses</t>
-  </si>
-  <si>
     <t>IL_RMS(A):</t>
   </si>
   <si>
     <t>FET</t>
   </si>
   <si>
-    <t>IPP051N15N5</t>
-  </si>
-  <si>
     <t>RDSon (ohm):</t>
   </si>
   <si>
@@ -419,9 +518,6 @@
     <t>Sync FET RMS Current(A):</t>
   </si>
   <si>
-    <t>SW Transition Losses (W):</t>
-  </si>
-  <si>
     <t>Total SW Transition Losses (W):</t>
   </si>
   <si>
@@ -431,9 +527,6 @@
     <t>Qoss(Coul.)</t>
   </si>
   <si>
-    <t>Qoss Losses Per FET:</t>
-  </si>
-  <si>
     <t>Ballpark Inductor Value:</t>
   </si>
   <si>
@@ -468,6 +561,33 @@
   </si>
   <si>
     <t>Design for MIC4102 for PWM input, add a not gate that can be DNP normally, but populated if need to change dot MIC4103</t>
+  </si>
+  <si>
+    <t>Total Qoss Losses (W)</t>
+  </si>
+  <si>
+    <t>SW Transition Losses (Boost) (W):</t>
+  </si>
+  <si>
+    <t>Qoss Losses Per (All) FET:</t>
+  </si>
+  <si>
+    <t>IPP075N15N3 G</t>
+  </si>
+  <si>
+    <t>Qrr losses per (Boost) FET: (W)</t>
+  </si>
+  <si>
+    <t>Total Qrr Losses:(W)</t>
+  </si>
+  <si>
+    <t>Losses &amp; Efficiency</t>
+  </si>
+  <si>
+    <t>Total Power Loss (W):</t>
+  </si>
+  <si>
+    <t>Estimated Efficiency:</t>
   </si>
 </sst>
 </file>
@@ -564,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -586,6 +706,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -905,11 +1034,543 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
+  <dimension ref="A1:T31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="13" max="13" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>80000</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="J7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="R7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <f>E7/E9</f>
+        <v>80000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <f>E13*0.5</f>
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <f>SQRT(E10)*E13</f>
+        <v>4.2107006542854597</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>48.72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9">
+        <f>(B16*E10)/(H8*E8)</f>
+        <v>9.9977499999999989E-5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9">
+        <f>SQRT(1-E10)*E13</f>
+        <v>4.2743420546325028</v>
+      </c>
+      <c r="R9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9">
+        <f>SUM(K31,K29,K27,K25,H26,H24)</f>
+        <v>18.801230181635848</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <f>(B18-B16)/B18</f>
+        <v>0.49249999999999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <f>(H8/2) + E13</f>
+        <v>7.5</v>
+      </c>
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10">
+        <f>((B19-S9)/B19)</f>
+        <v>0.97856090336886981</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>0.95</v>
+      </c>
+      <c r="M11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <f>E11*B19</f>
+        <v>833.11199999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <f>(B17/B8)</f>
+        <v>6</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <f>(E12/B8)/B18</f>
+        <v>2.8927499999999999</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="12">
+        <v>74437529203101</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <f>100*POWER(10,-6)</f>
+        <v>9.9999999999999991E-5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15">
+        <v>7.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f>B9</f>
+        <v>48.72</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16">
+        <v>2.2899999999999999E-3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16">
+        <f>70*POWER(10,-9)</f>
+        <v>7.0000000000000005E-8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f>B8*B10</f>
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17">
+        <v>9.4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17">
+        <f>56*POWER(10,-9)</f>
+        <v>5.6000000000000005E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>B13</f>
+        <v>96</v>
+      </c>
+      <c r="J18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18">
+        <f>179*POWER(10,-9)</f>
+        <v>1.79E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <f>B16*B17</f>
+        <v>876.96</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19">
+        <f>478*POWER(10,-9)</f>
+        <v>4.7800000000000002E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <f>(B16*E10)/(H15*E8)</f>
+        <v>2.9993250000000002</v>
+      </c>
+      <c r="J20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20">
+        <f>K17/N11</f>
+        <v>1.8666666666666668E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <f>E13+(0.5*H20)</f>
+        <v>7.4996625000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22">
+        <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
+        <v>6.0621499930279485</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23">
+        <f>POWER(H22,2)*H16</f>
+        <v>8.4156727211948459E-2</v>
+      </c>
+      <c r="J23" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23">
+        <f>POWER(K8,2)*K15</f>
+        <v>0.12765599999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24">
+        <f>H23*B8</f>
+        <v>0.25247018163584539</v>
+      </c>
+      <c r="J24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24">
+        <f>POWER(K9,2)*K15</f>
+        <v>0.13154400000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25">
+        <v>1.78E-2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25">
+        <f>SUM(K23:K24)*B8</f>
+        <v>0.77759999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26">
+        <f>H25*B8</f>
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>62</v>
+      </c>
+      <c r="K26">
+        <f>B18*E13*K20*E8</f>
+        <v>0.86016000000000015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J27" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27">
+        <f>K26*B8</f>
+        <v>2.5804800000000006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28">
+        <f>(K18/2)*B18*E8</f>
+        <v>0.68735999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J29" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29">
+        <f>K28*2*B8</f>
+        <v>4.1241599999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K30">
+        <f>K19*B18*E8</f>
+        <v>3.6710400000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J31" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31">
+        <f>K30*B8</f>
+        <v>11.013120000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:P7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
+    <hyperlink ref="H14" r:id="rId2" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/74437529203101?qs=f9yNj16SXrJ9N1gkF91A1Q%3D%3D" xr:uid="{C5698292-4A4E-457B-A7B0-B92AF5852830}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="E6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,11 +1580,12 @@
     <col min="7" max="7" width="32.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.453125" customWidth="1"/>
     <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
     <col min="13" max="13" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -932,14 +1594,14 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -947,7 +1609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -967,7 +1629,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -982,18 +1644,23 @@
       </c>
       <c r="H7" s="7"/>
       <c r="J7" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1015,20 +1682,20 @@
         <v>4.5</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K8">
         <f>SQRT(E10)*E13</f>
         <v>6.3160509814281891</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1042,21 +1709,28 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H9">
         <f>(B16*E10)/(H8*E8)</f>
         <v>2.3698370370370368E-5</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K9">
         <f>SQRT(1-E10)*E13</f>
         <v>6.4115130819487538</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S9">
+        <f>SUM(K31,K29,K27,K25,H26,H24)</f>
+        <v>40.475782132134938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1077,8 +1751,15 @@
         <f>(H8/2) + E13</f>
         <v>11.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10">
+        <f>((B19-S9)/B19)</f>
+        <v>0.95384534969424506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -1086,13 +1767,13 @@
         <v>0.95</v>
       </c>
       <c r="M11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="N11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1785,7 @@
         <v>833.11199999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1112,7 +1793,7 @@
         <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <f>(B17/E9)</f>
@@ -1127,7 +1808,7 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -1139,16 +1820,16 @@
         <v>30</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J14" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K14" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1160,13 +1841,13 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K15">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+        <v>7.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1175,17 +1856,17 @@
         <v>48.72</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16">
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K16">
-        <f>80*POWER(10,-9)</f>
-        <v>8.0000000000000002E-8</v>
+        <f>70*POWER(10,-9)</f>
+        <v>7.0000000000000005E-8</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1197,17 +1878,17 @@
         <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17">
         <v>14.7</v>
       </c>
       <c r="J17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K17">
-        <f>26*POWER(10,-9)</f>
-        <v>2.6000000000000001E-8</v>
+        <f>56*POWER(10,-9)</f>
+        <v>5.6000000000000005E-8</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1219,11 +1900,11 @@
         <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K18">
-        <f>299*POWER(10,-9)</f>
-        <v>2.9900000000000002E-7</v>
+        <f>179*POWER(10,-9)</f>
+        <v>1.79E-7</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1235,32 +1916,36 @@
         <v>876.96</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H19" s="6"/>
       <c r="J19" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="K19">
+        <f>478*POWER(10,-9)</f>
+        <v>4.7800000000000002E-7</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G20" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20">
         <f>(B16*E10)/(H15*E8)</f>
         <v>4.8473939393939389</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="K20">
         <f>K17/N11</f>
-        <v>8.6666666666666665E-9</v>
+        <v>1.8666666666666668E-8</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H21">
         <f>E13+(0.5*H20)</f>
@@ -1269,100 +1954,128 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G22" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H22">
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>9.1081338557159679</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H23">
         <f>POWER(H22,2)*H16</f>
         <v>0.21569106606746252</v>
       </c>
       <c r="J23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K23">
         <f>POWER(K8,2)*K15</f>
-        <v>0.17951624999999996</v>
+        <v>0.28722599999999993</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24">
         <f>H23*E9</f>
         <v>0.43138213213492504</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K24">
         <f>POWER(K9,2)*K15</f>
-        <v>0.18498375000000003</v>
+        <v>0.29597400000000007</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G25" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H25">
         <v>1.619</v>
       </c>
       <c r="J25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K25">
         <f>SUM(K23:K24)*E9</f>
-        <v>0.72899999999999998</v>
+        <v>1.1663999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G26" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H26">
         <f>H25*E9</f>
         <v>3.238</v>
       </c>
       <c r="J26" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="K26">
         <f>B18*E13*K20*E8</f>
-        <v>1.6848000000000001</v>
+        <v>3.6288000000000005</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J27" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K27">
         <f>K26*E9</f>
-        <v>3.3696000000000002</v>
+        <v>7.2576000000000009</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J28" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="K28">
         <f>(K18/2)*B18*E8</f>
-        <v>3.2292000000000001</v>
+        <v>1.9332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J29" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29">
+        <f>K28*2*E9</f>
+        <v>7.7328000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K30">
+        <f>K19*B18*E8</f>
+        <v>10.324800000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J31" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31">
+        <f>K30*E9</f>
+        <v>20.649600000000003</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="R7:T7"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="J13:K13"/>
@@ -1375,442 +2088,8 @@
     <mergeCell ref="M7:P7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K14" r:id="rId1" xr:uid="{1BC3AC28-62FC-4FF1-971A-2FE9F728A67C}"/>
-    <hyperlink ref="H14" r:id="rId2" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F195F5-CEE8-422B-8C7F-84AE41425DAF}">
-  <dimension ref="A1:N28"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
-    <col min="10" max="10" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>250000</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="J7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8">
-        <f>E7/E9</f>
-        <v>125000</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8">
-        <f>E13*0.5</f>
-        <v>3.6749999999999998</v>
-      </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8">
-        <f>SQRT(E10)*E13</f>
-        <v>4.7444045991040857</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>48.72</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9">
-        <f>(B16*E10)/(H8*E8)</f>
-        <v>1.26984126984127E-5</v>
-      </c>
-      <c r="J9" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9">
-        <f>SQRT(1-E10)*E13</f>
-        <v>5.613655226320903</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10">
-        <f>(B18-B16)/B18</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10">
-        <f>(H8/2) + E13</f>
-        <v>9.1875</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12">
-        <f>E11*B19</f>
-        <v>195.50999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>96</v>
-      </c>
-      <c r="D13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13">
-        <f>(B17/E9)</f>
-        <v>7.35</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="J13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14">
-        <f>(E12/E9)/B18</f>
-        <v>4.0731249999999992</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" t="s">
-        <v>27</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15">
-        <f>22*POWER(10,-6)</f>
-        <v>2.1999999999999999E-5</v>
-      </c>
-      <c r="J15" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="J16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K16">
-        <f>100*POWER(10,-9)</f>
-        <v>1.0000000000000001E-7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>14.7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17">
-        <v>14</v>
-      </c>
-      <c r="J17" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17">
-        <f>299*POWER(10,-9)</f>
-        <v>2.9900000000000002E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <f>B16*B17</f>
-        <v>205.79999999999998</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="6"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20">
-        <f>(B16*E10)/(H15*E8)</f>
-        <v>2.1212121212121215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21">
-        <f>E13+(0.5*H20)</f>
-        <v>8.4106060606060602</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22">
-        <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
-        <v>7.375463493137099</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23">
-        <f>POWER(H22,2)*H16</f>
-        <v>0.14143340052035505</v>
-      </c>
-      <c r="J23" t="s">
-        <v>46</v>
-      </c>
-      <c r="K23">
-        <f>POWER(K8,2)*K15</f>
-        <v>0.10129218750000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24">
-        <f>H23*E9</f>
-        <v>0.2828668010407101</v>
-      </c>
-      <c r="J24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K24">
-        <f>POWER(K9,2)*K15</f>
-        <v>0.14180906249999994</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K25">
-        <f>SUM(K23:K24)*E9</f>
-        <v>0.48620249999999987</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26">
-        <f>B18*E13*10*POWER(10,-9)*E8</f>
-        <v>0.2205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="J27" t="s">
-        <v>51</v>
-      </c>
-      <c r="K27">
-        <f>K26*E9</f>
-        <v>0.441</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="J28" t="s">
-        <v>54</v>
-      </c>
-      <c r="K28">
-        <f>(K17/2)*B18*E7</f>
-        <v>0.89700000000000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J13:K13"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1" display="https://www.coilcraft.com/en-us/products/power/shielded-inductors/high-current-flat-wire/ser/ser29xx/?skuId=10177" xr:uid="{B9E7DE04-5BE9-4709-A171-D1A5F059421D}"/>
-    <hyperlink ref="K14" r:id="rId2" xr:uid="{F6CD9C4B-A3B0-43B4-9E7F-23B8D2A7A72B}"/>
+    <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
+    <hyperlink ref="K14" r:id="rId2" xr:uid="{B236F431-81E3-4F17-BFE4-7EF14C8587EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
clean up design sheet
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C99689-4BE4-4098-92E0-900B7635296D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6B6878-E192-4EC6-8E9A-89ADC5DCC17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
@@ -93,6 +93,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{36FFA6F8-CCA9-41B8-B8DD-5F3C49DC1192}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby R:
+Design for MIC4102 for PWM input, add a not gate that can be DNP normally, but populated if need to change dot MIC4103</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G14" authorId="0" shapeId="0" xr:uid="{2D072AD2-0612-4777-9B01-271BE2591622}">
       <text>
         <r>
@@ -273,6 +288,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{E30345F2-9526-4B8A-90B1-45DC37C44DFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shelby R:
+Design for MIC4102 for PWM input, add a not gate that can be DNP normally, but populated if need to change dot MIC4103</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K14" authorId="0" shapeId="0" xr:uid="{99931F6F-1D2B-4A35-AFF8-CFF17CC6F28A}">
       <text>
         <r>
@@ -378,7 +408,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -558,9 +588,6 @@
   </si>
   <si>
     <t>MIC4102</t>
-  </si>
-  <si>
-    <t>Design for MIC4102 for PWM input, add a not gate that can be DNP normally, but populated if need to change dot MIC4103</t>
   </si>
   <si>
     <t>Total Qoss Losses (W)</t>
@@ -1038,7 +1065,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1123,7 +1150,7 @@
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="R7" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -1157,10 +1184,10 @@
         <v>4.2107006542854597</v>
       </c>
       <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="O8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
@@ -1191,11 +1218,11 @@
         <v>4.2743420546325028</v>
       </c>
       <c r="R9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S9">
         <f>SUM(K31,K29,K27,K25,H26,H24)</f>
-        <v>18.801230181635848</v>
+        <v>21.073461816358456</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
@@ -1220,11 +1247,11 @@
         <v>7.5</v>
       </c>
       <c r="R10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S10">
         <f>((B19-S9)/B19)</f>
-        <v>0.97856090336886981</v>
+        <v>0.97596987112712275</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
@@ -1294,7 +1321,7 @@
         <v>27</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
@@ -1327,7 +1354,7 @@
         <v>31</v>
       </c>
       <c r="H16">
-        <v>2.2899999999999999E-3</v>
+        <v>2.29E-2</v>
       </c>
       <c r="J16" t="s">
         <v>47</v>
@@ -1439,7 +1466,7 @@
       </c>
       <c r="H23">
         <f>POWER(H22,2)*H16</f>
-        <v>8.4156727211948459E-2</v>
+        <v>0.84156727211948457</v>
       </c>
       <c r="J23" t="s">
         <v>42</v>
@@ -1455,7 +1482,7 @@
       </c>
       <c r="H24">
         <f>H23*B8</f>
-        <v>0.25247018163584539</v>
+        <v>2.5247018163584536</v>
       </c>
       <c r="J24" t="s">
         <v>44</v>
@@ -1489,7 +1516,7 @@
         <v>5.3400000000000003E-2</v>
       </c>
       <c r="J26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K26">
         <f>B18*E13*K20*E8</f>
@@ -1507,7 +1534,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K28">
         <f>(K18/2)*B18*E8</f>
@@ -1516,7 +1543,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K29">
         <f>K28*2*B8</f>
@@ -1525,7 +1552,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K30">
         <f>K19*B18*E8</f>
@@ -1534,7 +1561,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K31">
         <f>K30*B8</f>
@@ -1558,10 +1585,11 @@
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
     <hyperlink ref="H14" r:id="rId2" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/74437529203101?qs=f9yNj16SXrJ9N1gkF91A1Q%3D%3D" xr:uid="{C5698292-4A4E-457B-A7B0-B92AF5852830}"/>
+    <hyperlink ref="N8" r:id="rId3" xr:uid="{60702E27-9954-4BEA-853A-9CFF3E8394F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1569,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="E6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1655,7 +1683,7 @@
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="R7" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -1689,10 +1717,10 @@
         <v>6.3160509814281891</v>
       </c>
       <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="O8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
@@ -1723,7 +1751,7 @@
         <v>6.4115130819487538</v>
       </c>
       <c r="R9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S9">
         <f>SUM(K31,K29,K27,K25,H26,H24)</f>
@@ -1752,7 +1780,7 @@
         <v>11.25</v>
       </c>
       <c r="R10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S10">
         <f>((B19-S9)/B19)</f>
@@ -1826,7 +1854,7 @@
         <v>27</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
@@ -2021,7 +2049,7 @@
         <v>3.238</v>
       </c>
       <c r="J26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K26">
         <f>B18*E13*K20*E8</f>
@@ -2039,7 +2067,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K28">
         <f>(K18/2)*B18*E8</f>
@@ -2048,7 +2076,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K29">
         <f>K28*2*E9</f>
@@ -2057,7 +2085,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K30">
         <f>K19*B18*E8</f>
@@ -2066,7 +2094,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="J31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K31">
         <f>K30*E9</f>
@@ -2090,9 +2118,10 @@
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
     <hyperlink ref="K14" r:id="rId2" xr:uid="{B236F431-81E3-4F17-BFE4-7EF14C8587EF}"/>
+    <hyperlink ref="N8" r:id="rId3" xr:uid="{DC87458B-4210-4677-9A1D-A7107BA34E04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add alternate gate drive components
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6B6878-E192-4EC6-8E9A-89ADC5DCC17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A74A49-EC38-47D3-AEF0-282F5D95A4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
@@ -408,7 +408,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -615,6 +615,24 @@
   </si>
   <si>
     <t>Estimated Efficiency:</t>
+  </si>
+  <si>
+    <t>MAX5063DASA+</t>
+  </si>
+  <si>
+    <t>Alt Part 1:</t>
+  </si>
+  <si>
+    <t>Alt Part 2:</t>
+  </si>
+  <si>
+    <t>MIC4103YM</t>
+  </si>
+  <si>
+    <t>Alt Part 3:</t>
+  </si>
+  <si>
+    <t>MAX15019BASA+</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1217,6 +1235,12 @@
         <f>SQRT(1-E10)*E13</f>
         <v>4.2743420546325028</v>
       </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="R9" t="s">
         <v>67</v>
       </c>
@@ -1246,6 +1270,12 @@
         <f>(H8/2) + E13</f>
         <v>7.5</v>
       </c>
+      <c r="M10" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" t="s">
+        <v>72</v>
+      </c>
       <c r="R10" t="s">
         <v>68</v>
       </c>
@@ -1262,10 +1292,10 @@
         <v>0.95</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
+        <v>73</v>
+      </c>
+      <c r="N11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -1279,6 +1309,12 @@
         <f>E11*B19</f>
         <v>833.11199999999997</v>
       </c>
+      <c r="M12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1434,7 +1470,7 @@
         <v>58</v>
       </c>
       <c r="K20">
-        <f>K17/N11</f>
+        <f>K17/N12</f>
         <v>1.8666666666666668E-8</v>
       </c>
     </row>
@@ -1586,10 +1622,11 @@
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
     <hyperlink ref="H14" r:id="rId2" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/74437529203101?qs=f9yNj16SXrJ9N1gkF91A1Q%3D%3D" xr:uid="{C5698292-4A4E-457B-A7B0-B92AF5852830}"/>
     <hyperlink ref="N8" r:id="rId3" xr:uid="{60702E27-9954-4BEA-853A-9CFF3E8394F2}"/>
+    <hyperlink ref="N9" r:id="rId4" xr:uid="{7D8684E0-555C-4A45-AC83-3F8666047795}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add parts list of components to make in library
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669EC83A-670C-404B-8B86-3F87B1F16BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A2B9F9-B301-4100-848E-C6F1E39636FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi_String_Single_phase" sheetId="3" r:id="rId1"/>
-    <sheet name="Original_Multiphase" sheetId="1" r:id="rId2"/>
-    <sheet name="POL_Power_Breakdown" sheetId="4" r:id="rId3"/>
+    <sheet name="Library_Parts_To_Make" sheetId="5" r:id="rId2"/>
+    <sheet name="Original_Multiphase" sheetId="1" r:id="rId3"/>
+    <sheet name="POL_Power_Breakdown" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -250,6 +251,31 @@
     <author>Windows PC</author>
   </authors>
   <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{EE5894B5-F449-47EE-BD0A-0D3082B357D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>S. Riggleman:
+Chose as opposed to D2-Pak package due to chip shortage - 4200 available on Mouser and interchangable if necessary</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Windows PC</author>
+  </authors>
+  <commentList>
     <comment ref="E7" authorId="0" shapeId="0" xr:uid="{5FBF964B-8E52-42FE-A1BE-4091C63B5871}">
       <text>
         <r>
@@ -423,7 +449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="129">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -768,13 +794,55 @@
   </si>
   <si>
     <t>1.75 @ 100hz</t>
+  </si>
+  <si>
+    <t>Power Inductor:</t>
+  </si>
+  <si>
+    <t>MOSFET:</t>
+  </si>
+  <si>
+    <t>Gate Driver:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrolytic Cap: </t>
+  </si>
+  <si>
+    <t>12V Regulator:</t>
+  </si>
+  <si>
+    <t>MAX5033CUSA+</t>
+  </si>
+  <si>
+    <t>10uF ceramic:</t>
+  </si>
+  <si>
+    <t>C3216X6S2A106K160AC</t>
+  </si>
+  <si>
+    <t>.1uF Ceramic:</t>
+  </si>
+  <si>
+    <t>CGA4J3X7T2E104K125AA</t>
+  </si>
+  <si>
+    <t>1uF Ceramic:</t>
+  </si>
+  <si>
+    <t>GMC31X7R105K100NT</t>
+  </si>
+  <si>
+    <t>SRR1260A-561K</t>
+  </si>
+  <si>
+    <t>Buck Inductor:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,13 +910,24 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF444444"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -864,7 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -875,10 +954,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -887,17 +977,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -931,8 +1016,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161980</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -951,7 +1036,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -996,8 +1081,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>15610</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -1016,7 +1101,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -1061,8 +1146,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>126870</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="8" name="Ink 7">
@@ -1081,7 +1166,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="8" name="Ink 7">
@@ -1126,8 +1211,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>133330</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -1146,7 +1231,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -1191,8 +1276,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>50720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="14" name="Ink 13">
@@ -1211,7 +1296,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="14" name="Ink 13">
@@ -1383,10 +1468,6 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="638.79">372 550 24575</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1957.43">442 3 24575,'33'-2'0,"25"1"0,-54 1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1 0 0,4 2 0,-6-1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,0 5 0,0 7 0,0 0 0,-4 21 0,2-29 0,2-7 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,2 1 0,3 2 0,0 0 0,1 0 0,-1 0 0,0 1 0,0 0 0,-1 1 0,1-1 0,4 6 0,-7-6 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,2 10 0,-3-12 0,2 5 0,-1 1 0,-1 0 0,1-1 0,-2 1 0,0 9 0,1-16 0,-1 0 0,1 0 0,0-1 0,-1 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,-2 1 0,-14 0-100,0 0-1,-24-2 1,27 0-964,-6 0-5762</inkml:trace>
 </inkml:ink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1688,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView topLeftCell="J4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1707,25 +1788,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1755,21 +1836,21 @@
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1781,29 +1862,29 @@
       <c r="E7">
         <v>80000</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="J7" s="6" t="s">
+      <c r="H7" s="11"/>
+      <c r="J7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="6" t="s">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="R7" s="6" t="s">
+      <c r="N7" s="10"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="R7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="6"/>
-      <c r="U7" s="6" t="s">
+      <c r="S7" s="10"/>
+      <c r="U7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="7"/>
+      <c r="V7" s="11"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1956,26 +2037,26 @@
         <f>(B17/B8)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="J13" s="6" t="s">
+      <c r="H13" s="10"/>
+      <c r="J13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="M13" s="6" t="s">
+      <c r="K13" s="11"/>
+      <c r="M13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="6"/>
-      <c r="R13" s="6" t="s">
+      <c r="N13" s="10"/>
+      <c r="R13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="6"/>
-      <c r="U13" s="6" t="s">
+      <c r="S13" s="10"/>
+      <c r="U13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="7"/>
+      <c r="V13" s="11"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
@@ -1988,13 +2069,13 @@
       <c r="G14" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="7">
         <v>74437529203101</v>
       </c>
       <c r="J14" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="M14" t="s">
@@ -2130,10 +2211,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="10"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -2175,18 +2256,18 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>6.0621499930279485</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="M22" s="6" t="s">
+      <c r="K22" s="11"/>
+      <c r="M22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="7"/>
-      <c r="U22" s="6" t="s">
+      <c r="N22" s="11"/>
+      <c r="U22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="V22" s="7"/>
+      <c r="V22" s="11"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G23" s="5" t="s">
@@ -2354,24 +2435,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U22:V22"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="R13:S13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="G1:I1"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
@@ -2387,6 +2468,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81E0D2E-BF7B-44F8-984B-BF407D8DCAAB}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="7">
+        <v>74437529203101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/74437529203101?qs=f9yNj16SXrJ9N1gkF91A1Q%3D%3D" xr:uid="{9EFE9F91-55C8-4A2B-B2B7-EC6495F07CAD}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.mouser.com/ProductDetail/Wurth-Elektronik/74437529203101?qs=f9yNj16SXrJ9N1gkF91A1Q%3D%3D" xr:uid="{7819EBCA-EB69-4C1E-AF42-5A095F5213F8}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{8C47C7BC-E5EA-4A7F-8553-CD6E65C5C5B7}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{A90CD90E-1F29-4EE6-A4EC-961DFAE8E9CF}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{9B171363-0FC1-40E1-87D2-62020BC77A86}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{48522BF1-C64B-4936-9506-19A38019129B}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{43196D4C-8373-4379-8D00-BD043B7B5E79}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{0388FA5F-BAD6-409E-BFE6-BAD8991DB93F}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC31X7R105K100NT/12697998" xr:uid="{5FA621FA-8195-49BE-A329-951A02254B72}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{731786E7-E83A-40B9-BB1A-68221AAA2B3B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC921004-1896-46EC-BBDE-67F57C6F91C3}">
   <dimension ref="A1:P31"/>
   <sheetViews>
@@ -2407,25 +2599,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -2455,21 +2647,21 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -2481,21 +2673,21 @@
       <c r="E7">
         <v>450000</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="J7" s="6" t="s">
+      <c r="H7" s="11"/>
+      <c r="J7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7" t="s">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -2634,18 +2826,18 @@
         <f>(B17/E9)</f>
         <v>9</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="J13" s="6" t="s">
+      <c r="H13" s="10"/>
+      <c r="J13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="M13" s="6" t="s">
+      <c r="K13" s="11"/>
+      <c r="M13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="6"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
@@ -2664,7 +2856,7 @@
       <c r="J14" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="M14" t="s">
@@ -2766,10 +2958,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="10"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -2811,14 +3003,14 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>9.1081338557159679</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="M22" s="6" t="s">
+      <c r="K22" s="11"/>
+      <c r="M22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="6"/>
+      <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G23" s="5" t="s">
@@ -2944,6 +3136,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:P7"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="M22:N22"/>
@@ -2951,12 +3149,6 @@
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:P7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>
@@ -2970,7 +3162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585350FB-4F44-44C9-BD54-CA099149966A}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -3018,7 +3210,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="8" t="s">
         <v>89</v>
       </c>
       <c r="E2">

</xml_diff>

<commit_message>
add CAN transceiver and LDO to list
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A2B9F9-B301-4100-848E-C6F1E39636FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90F4DE2-F7C2-4385-9564-5F379766A775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
@@ -449,7 +449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="133">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -836,13 +836,25 @@
   </si>
   <si>
     <t>Buck Inductor:</t>
+  </si>
+  <si>
+    <t>LDO:</t>
+  </si>
+  <si>
+    <t>ST715CR</t>
+  </si>
+  <si>
+    <t>CAN Transciever:</t>
+  </si>
+  <si>
+    <t>IL 41050TE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -910,24 +922,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF444444"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -943,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -976,12 +977,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2469,10 +2464,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81E0D2E-BF7B-44F8-984B-BF407D8DCAAB}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2481,10 +2476,10 @@
     <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="7"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -2492,7 +2487,7 @@
         <v>74437529203101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -2500,7 +2495,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -2508,7 +2503,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -2516,7 +2511,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -2524,7 +2519,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2532,7 +2527,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -2540,7 +2535,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -2548,16 +2543,45 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2571,10 +2595,12 @@
     <hyperlink ref="B10" r:id="rId8" xr:uid="{0388FA5F-BAD6-409E-BFE6-BAD8991DB93F}"/>
     <hyperlink ref="B11" r:id="rId9" display="https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC31X7R105K100NT/12697998" xr:uid="{5FA621FA-8195-49BE-A329-951A02254B72}"/>
     <hyperlink ref="B12" r:id="rId10" xr:uid="{731786E7-E83A-40B9-BB1A-68221AAA2B3B}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{BAEA17AE-4224-423B-B603-CDC00085BD0F}"/>
+    <hyperlink ref="B14:D14" r:id="rId12" display="IL 41050TE" xr:uid="{2AA44490-8FF9-4866-BCB1-D2ABEC508341}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
work on nucleo schematic
</commit_message>
<xml_diff>
--- a/MPPT/design/Converter_calculations.xlsx
+++ b/MPPT/design/Converter_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows PC\Desktop\Badgerloop\git_repos\solar_car_hardware\MPPT\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B1400-AB22-4F51-B795-0F3DE5FF1C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD83118-037C-4BA8-B5E2-D914471F614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{632D32AA-A087-40DE-B097-47254B8CA429}"/>
   </bookViews>
   <sheets>
     <sheet name="Multi_String_Single_phase" sheetId="3" r:id="rId1"/>
@@ -449,7 +449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="138">
   <si>
     <t>Multiphase Boost Converter Design</t>
   </si>
@@ -848,6 +848,21 @@
   </si>
   <si>
     <t>IL 41050TE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCU </t>
+  </si>
+  <si>
+    <t>Nucleo-Fk3038</t>
+  </si>
+  <si>
+    <t>P/N:</t>
+  </si>
+  <si>
+    <t>Top current draw:</t>
+  </si>
+  <si>
+    <t>Power Consumed</t>
   </si>
 </sst>
 </file>
@@ -963,12 +978,6 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -976,6 +985,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1762,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0EE43-D721-4343-AE35-2BE488142AE4}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView topLeftCell="J4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1782,28 +1797,28 @@
     <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="G1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1814,40 +1829,40 @@
         <v>67</v>
       </c>
       <c r="H3">
-        <f>SUM(K31,K29,K27,K25,H26,H24,N23)</f>
-        <v>21.443733816358456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+        <f>SUM(K31,K29,K27,K25,H26,H24,N23,Y23)</f>
+        <v>25.043733816358454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G4" t="s">
         <v>68</v>
       </c>
       <c r="H4">
         <f>((B19-H3)/B19)</f>
-        <v>0.97554764890490053</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+        <v>0.97144255859291362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1857,31 +1872,34 @@
       <c r="E7">
         <v>80000</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="J7" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="J7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="12" t="s">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="12"/>
+      <c r="N7" s="10"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="12"/>
-      <c r="U7" s="12" t="s">
+      <c r="S7" s="10"/>
+      <c r="U7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="13"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V7" s="11"/>
+      <c r="X7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1929,8 +1947,14 @@
         <f>E14*SQRT(E10/(1-E10))</f>
         <v>2.849679356962814</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X8" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1963,8 +1987,14 @@
       <c r="N9" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X9" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1991,8 +2021,14 @@
       <c r="N10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -2006,7 +2042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2018,7 +2054,7 @@
         <v>833.11199999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2032,28 +2068,28 @@
         <f>(B17/B8)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="J13" s="12" t="s">
+      <c r="H13" s="10"/>
+      <c r="J13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="M13" s="12" t="s">
+      <c r="K13" s="11"/>
+      <c r="M13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="12"/>
-      <c r="R13" s="12" t="s">
+      <c r="N13" s="10"/>
+      <c r="R13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="12"/>
-      <c r="U13" s="12" t="s">
+      <c r="S13" s="10"/>
+      <c r="U13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="13"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V13" s="11"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -2089,7 +2125,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2120,7 +2156,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2148,7 +2184,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2212,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2198,7 +2234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2206,10 +2242,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="10"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -2218,7 +2254,7 @@
         <v>4.7800000000000002E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G20" s="5" t="s">
         <v>34</v>
       </c>
@@ -2234,7 +2270,7 @@
         <v>1.8666666666666668E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G21" s="5" t="s">
         <v>35</v>
       </c>
@@ -2243,7 +2279,7 @@
         <v>7.4996625000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G22" s="5" t="s">
         <v>38</v>
       </c>
@@ -2251,20 +2287,24 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>6.0621499930279485</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="M22" s="12" t="s">
+      <c r="K22" s="11"/>
+      <c r="M22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="13"/>
-      <c r="U22" s="12" t="s">
+      <c r="N22" s="11"/>
+      <c r="U22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="V22" s="13"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V22" s="11"/>
+      <c r="X22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y22" s="11"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G23" s="5" t="s">
         <v>36</v>
       </c>
@@ -2293,8 +2333,15 @@
         <f>V18*V15</f>
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="X23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y23">
+        <f>Y10*Y9</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G24" s="5" t="s">
         <v>37</v>
       </c>
@@ -2324,7 +2371,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G25" s="5" t="s">
         <v>52</v>
       </c>
@@ -2346,7 +2393,7 @@
         <v>9.2322972656249998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="G26" s="5" t="s">
         <v>53</v>
       </c>
@@ -2369,7 +2416,7 @@
         <v>5.6999999999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="J27" t="s">
         <v>46</v>
       </c>
@@ -2385,7 +2432,7 @@
         <v>0.11399999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="J28" t="s">
         <v>62</v>
       </c>
@@ -2401,7 +2448,7 @@
         <v>0.11437322812966706</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="J29" t="s">
         <v>60</v>
       </c>
@@ -2410,7 +2457,7 @@
         <v>4.1241599999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="J30" t="s">
         <v>64</v>
       </c>
@@ -2419,7 +2466,7 @@
         <v>3.6710400000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="J31" t="s">
         <v>65</v>
       </c>
@@ -2429,7 +2476,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="U13:V13"/>
@@ -2438,16 +2496,6 @@
     <mergeCell ref="R13:S13"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{0659C5BF-1BC6-4969-8EFC-68C7F5058594}"/>
@@ -2466,7 +2514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81E0D2E-BF7B-44F8-984B-BF407D8DCAAB}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -2625,25 +2673,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="G1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -2673,21 +2721,21 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -2699,21 +2747,21 @@
       <c r="E7">
         <v>450000</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="J7" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="J7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13" t="s">
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -2852,18 +2900,18 @@
         <f>(B17/E9)</f>
         <v>9</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="J13" s="12" t="s">
+      <c r="H13" s="10"/>
+      <c r="J13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="M13" s="12" t="s">
+      <c r="K13" s="11"/>
+      <c r="M13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="12"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
@@ -2984,10 +3032,10 @@
         <f>B16*B17</f>
         <v>876.96</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="10"/>
       <c r="J19" t="s">
         <v>54</v>
       </c>
@@ -3029,14 +3077,14 @@
         <f>SQRT(POWER(E13,2) + POWER(H20/SQRT(12),2))</f>
         <v>9.1081338557159679</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="M22" s="12" t="s">
+      <c r="K22" s="11"/>
+      <c r="M22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="12"/>
+      <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G23" s="5" t="s">
@@ -3162,12 +3210,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:N5"/>
@@ -3175,6 +3217,12 @@
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{D2437223-55EC-4ADD-8FEA-0B638A64EC0B}"/>

</xml_diff>